<commit_message>
- added .gitignore - tried some things
</commit_message>
<xml_diff>
--- a/Data/Fulldata.xlsx
+++ b/Data/Fulldata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Bachlor-Arbeit\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Bachelor-Arbeit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B98ADC-C2CB-420E-8B27-40142C101850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A24078-28AF-469C-B9BF-5240697C6554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1040,15 +1040,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G577"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A552" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="0.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
     <col min="5" max="5" width="0.140625" customWidth="1"/>
     <col min="6" max="6" width="157.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
final commit juhu fertig !!!
</commit_message>
<xml_diff>
--- a/Data/Fulldata.xlsx
+++ b/Data/Fulldata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Uni\Bachelor-Arbeit\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BA4017-010E-449C-91B9-D2CB8E268216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7058B12-BE0D-41BF-B350-7DA6A98584F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>